<commit_message>
sql scripts first init
</commit_message>
<xml_diff>
--- a/Stuff/Draft.xlsx
+++ b/Stuff/Draft.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PGarlej\Desktop\Stuff\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="JavaObjects" sheetId="1" r:id="rId1"/>
     <sheet name="MySQL tables" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Object</t>
   </si>
@@ -144,9 +139,6 @@
     </r>
   </si>
   <si>
-    <t>Name   :   VARCHAR</t>
-  </si>
-  <si>
     <t>Maker   :   VARCHAR</t>
   </si>
   <si>
@@ -204,9 +196,6 @@
     <t>ObjectDetailsID   :   INT() (fk)</t>
   </si>
   <si>
-    <t>ObjectID   :   INT() (fk)</t>
-  </si>
-  <si>
     <t>InspectionFormID   :   INT() (fk)</t>
   </si>
   <si>
@@ -229,13 +218,19 @@
   </si>
   <si>
     <t>SerialNumber   :   VARCHAR (unique with InspectionFormID)</t>
+  </si>
+  <si>
+    <t>ObjectID   :   INT() (fk; unique with Name)</t>
+  </si>
+  <si>
+    <t>Name   :   VARCHAR (unique with ObjectID)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,50 +355,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Łącznik prosty 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1762125" y="257175"/>
-          <a:ext cx="628650" cy="581025"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>1771650</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -447,8 +398,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
@@ -456,7 +407,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -465,8 +416,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="5734050" y="476250"/>
-          <a:ext cx="647700" cy="752475"/>
+          <a:off x="7038975" y="476250"/>
+          <a:ext cx="619125" cy="752476"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -491,16 +442,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -509,8 +460,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="5724525" y="466725"/>
-          <a:ext cx="3162300" cy="2295525"/>
+          <a:off x="7029450" y="476250"/>
+          <a:ext cx="3133725" cy="2286001"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -714,7 +665,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,7 +700,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -926,21 +877,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -952,7 +903,7 @@
     <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -974,7 +925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -997,7 +948,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1020,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1061,7 +1012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1026,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="G8" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="G9" t="s">
         <v>25</v>
       </c>
@@ -1091,37 +1042,37 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="G10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="G11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="G12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="G13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="G14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1133,20 +1084,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
@@ -1158,7 +1109,7 @@
     <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1177,172 +1128,170 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="I9" t="s">
         <v>41</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
-        <v>42</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="I11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="I12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="I13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
+    <row r="14" spans="1:13">
+      <c r="I14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="I15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>

</xml_diff>

<commit_message>
created entities for objects and forms
</commit_message>
<xml_diff>
--- a/Stuff/Draft.xlsx
+++ b/Stuff/Draft.xlsx
@@ -20,23 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Object</t>
   </si>
   <si>
-    <t>ObjectDetails</t>
-  </si>
-  <si>
     <t>List&lt;InspectionForm&gt;</t>
   </si>
   <si>
     <t>InspectionForm</t>
   </si>
   <si>
-    <t>InspectionStep</t>
-  </si>
-  <si>
     <t>List&lt;InspectionStep&gt;</t>
   </si>
   <si>
@@ -49,83 +43,119 @@
     <t>List&lt;InspectionResult&gt;</t>
   </si>
   <si>
-    <t>ID   :   int</t>
-  </si>
-  <si>
-    <t>Name   :   String</t>
-  </si>
-  <si>
-    <t>Maker   :   String</t>
-  </si>
-  <si>
-    <t>ObjectDetailsID   :   int</t>
-  </si>
-  <si>
-    <t>Description   :   String</t>
-  </si>
-  <si>
-    <t>ObjectID   :   int</t>
-  </si>
-  <si>
-    <t>Details   :   String</t>
-  </si>
-  <si>
-    <t>SerialNumber   :   String</t>
-  </si>
-  <si>
-    <t>Result   :   int</t>
-  </si>
-  <si>
-    <t>FileName   :   String</t>
-  </si>
-  <si>
-    <t>StepNumber   :   int</t>
-  </si>
-  <si>
-    <t>CreationDate   :   Date</t>
-  </si>
-  <si>
-    <t>Notes   :   String</t>
-  </si>
-  <si>
-    <t>CreationHour   :   Date</t>
-  </si>
-  <si>
-    <t>CompletionDate   :   Date</t>
-  </si>
-  <si>
-    <t>InspectionID   :   int</t>
-  </si>
-  <si>
-    <t>CompletionHour   :   Date</t>
-  </si>
-  <si>
-    <t>Inspector   :   String</t>
-  </si>
-  <si>
-    <t>Place   :   String</t>
-  </si>
-  <si>
-    <t>Batch   :   int</t>
-  </si>
-  <si>
-    <t>MainResult   :   int</t>
-  </si>
-  <si>
-    <t>InspectionFormID   :   int</t>
-  </si>
-  <si>
-    <t>InspectionResultID   :   int</t>
-  </si>
-  <si>
     <t>List&lt;FaultPicture&gt;</t>
   </si>
   <si>
     <t>FaultPicture</t>
   </si>
   <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>ObjectDetail</t>
+  </si>
+  <si>
+    <t>object_detail_id   :   INT() (fk)</t>
+  </si>
+  <si>
+    <t>name   :   VARCHAR (unique)</t>
+  </si>
+  <si>
+    <t>id   :   INT() (pk)</t>
+  </si>
+  <si>
+    <t>maker   :   VARCHAR</t>
+  </si>
+  <si>
+    <t>description   :   TEXT</t>
+  </si>
+  <si>
+    <t>name   :   VARCHAR (unique with ObjectID)</t>
+  </si>
+  <si>
+    <t>object_id   :   INT() (fk; unique with Name)</t>
+  </si>
+  <si>
+    <t>details   :   TEXT</t>
+  </si>
+  <si>
+    <t>step_number   :   INT()</t>
+  </si>
+  <si>
+    <t>inspection_form_id   :   INT() (fk)</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>object_detail</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>number   :   int</t>
+  </si>
+  <si>
+    <t>number   :   INT()</t>
+  </si>
+  <si>
+    <t>id   :   int</t>
+  </si>
+  <si>
+    <t>name   :   String</t>
+  </si>
+  <si>
+    <t>objectDetail</t>
+  </si>
+  <si>
+    <t>description   :   String</t>
+  </si>
+  <si>
+    <t>maker   :   String</t>
+  </si>
+  <si>
+    <t>details   :   String</t>
+  </si>
+  <si>
+    <t>serialNumber   :   String</t>
+  </si>
+  <si>
+    <t>creationDate   :   Date</t>
+  </si>
+  <si>
+    <t>creationHour   :   Date</t>
+  </si>
+  <si>
+    <t>completionDate   :   Date</t>
+  </si>
+  <si>
+    <t>completionHour   :   Date</t>
+  </si>
+  <si>
+    <t>inspector   :   String</t>
+  </si>
+  <si>
+    <t>place   :   String</t>
+  </si>
+  <si>
+    <t>batch   :   int</t>
+  </si>
+  <si>
+    <t>mainResult   :   int</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Completed   :   </t>
+      <t xml:space="preserve">completed   :   </t>
     </r>
     <r>
       <rPr>
@@ -139,98 +169,74 @@
     </r>
   </si>
   <si>
-    <t>Maker   :   VARCHAR</t>
-  </si>
-  <si>
-    <t>FileName   :   VARCHAR</t>
-  </si>
-  <si>
-    <t>Inspector   :   VARCHAR</t>
-  </si>
-  <si>
-    <t>Place   :   VARCHAR</t>
-  </si>
-  <si>
-    <t>CreationDate   :   DATE()</t>
-  </si>
-  <si>
-    <t>CompletionDate   :   DATE()</t>
-  </si>
-  <si>
-    <t>CompletionHour   :   TIME()</t>
-  </si>
-  <si>
-    <t>CreationHour   :   TIME()</t>
-  </si>
-  <si>
-    <t>Result   :   INT()</t>
-  </si>
-  <si>
-    <t>StepNumber   :   INT()</t>
-  </si>
-  <si>
-    <t>Batch   :   INT()</t>
-  </si>
-  <si>
-    <t>MainResult   :   INT()</t>
-  </si>
-  <si>
-    <t>Completed   :   TINYINT()(1)</t>
-  </si>
-  <si>
-    <t>Description   :   TEXT</t>
-  </si>
-  <si>
-    <t>Details   :   TEXT</t>
-  </si>
-  <si>
-    <t>Notes   :   TEXT</t>
-  </si>
-  <si>
-    <t>Name   :   VARCHAR (unique)</t>
-  </si>
-  <si>
-    <t>ID   :   INT() (pk)</t>
-  </si>
-  <si>
-    <t>ObjectDetailsID   :   INT() (fk)</t>
-  </si>
-  <si>
-    <t>InspectionFormID   :   INT() (fk)</t>
-  </si>
-  <si>
-    <t>InspectionID   :   INT() (fk)</t>
-  </si>
-  <si>
-    <t>InspectionResultID   :   INT() (fk)</t>
-  </si>
-  <si>
-    <t>Form</t>
-  </si>
-  <si>
-    <t>Step</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>InspectionFormID   :   INT() (fk; unique with SerialNumber)</t>
-  </si>
-  <si>
-    <t>SerialNumber   :   VARCHAR (unique with InspectionFormID)</t>
-  </si>
-  <si>
-    <t>ObjectID   :   INT() (fk; unique with Name)</t>
-  </si>
-  <si>
-    <t>Name   :   VARCHAR (unique with ObjectID)</t>
+    <t>result   :   int</t>
+  </si>
+  <si>
+    <t>notes   :   String</t>
+  </si>
+  <si>
+    <t>stepNumber   :   int</t>
+  </si>
+  <si>
+    <t>inspection</t>
+  </si>
+  <si>
+    <t>fileName   :   String</t>
+  </si>
+  <si>
+    <t>serial_number   :   VARCHAR (unique with InspectionFormID)</t>
+  </si>
+  <si>
+    <t>creation_date   :   DATE()</t>
+  </si>
+  <si>
+    <t>creation_hour   :   TIME()</t>
+  </si>
+  <si>
+    <t>completion_date   :   DATE()</t>
+  </si>
+  <si>
+    <t>completion_hour   :   TIME()</t>
+  </si>
+  <si>
+    <t>inspector   :   VARCHAR</t>
+  </si>
+  <si>
+    <t>place   :   VARCHAR</t>
+  </si>
+  <si>
+    <t>batch   :   INT()</t>
+  </si>
+  <si>
+    <t>main_result   :   INT()</t>
+  </si>
+  <si>
+    <t>completed   :   TINYINT()(1)</t>
+  </si>
+  <si>
+    <t>inspection_form_id   :   INT() (fk; unique with SerialNumber)</t>
+  </si>
+  <si>
+    <t>result   :   INT()</t>
+  </si>
+  <si>
+    <t>notes   :   TEXT</t>
+  </si>
+  <si>
+    <t>inspection_id   :   INT() (fk)</t>
+  </si>
+  <si>
+    <t>file_name   :   VARCHAR</t>
+  </si>
+  <si>
+    <t>inspection_result_id   :   INT() (fk)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +270,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,10 +299,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -877,7 +892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -888,7 +903,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -908,173 +923,173 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
+        <v>37</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="G8" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="G9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="G10" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="G11" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="G12" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="G13" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="G14" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="G15" s="2" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="G16" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1088,7 +1103,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,11 +1126,11 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1130,66 +1145,66 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1198,91 +1213,91 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" t="s">
         <v>61</v>
       </c>
-      <c r="K5" t="s">
-        <v>43</v>
-      </c>
       <c r="M5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="I8" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:13">
       <c r="I9" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:13">
       <c r="I10" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="I11" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="I12" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="I13" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="I14" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:13">

</xml_diff>

<commit_message>
added sql scripts for inspection tables
</commit_message>
<xml_diff>
--- a/Stuff/Draft.xlsx
+++ b/Stuff/Draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JavaObjects" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
     <t>inspection_id   :   INT() (fk)</t>
   </si>
   <si>
-    <t>file_name   :   VARCHAR</t>
-  </si>
-  <si>
     <t>form_id   :   INT() (fk; unique with SerialNumber)</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>ItemDetail</t>
+  </si>
+  <si>
+    <t>file_name   :   TEXT</t>
   </si>
 </sst>
 </file>
@@ -895,7 +895,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -923,10 +923,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -968,7 +968,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
@@ -1015,7 +1015,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -1105,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1228,7 +1228,7 @@
         <v>55</v>
       </c>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1246,7 +1246,7 @@
         <v>56</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1259,7 +1259,7 @@
         <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1305,7 +1305,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="I15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" s="2"/>
     </row>

</xml_diff>